<commit_message>
Removed menu «Долги» for users Armines (id=486) and Lusines (id=484)
</commit_message>
<xml_diff>
--- a/doc/Reports_Permissions.xlsx
+++ b/doc/Reports_Permissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web\webroot\test\files\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176EA7C4-48D0-4F6E-BE81-8A2EB368E521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5382EE5-818E-4A0B-895F-EA3BB60431D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -591,7 +591,7 @@
   <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1418,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="6"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
@@ -1427,7 +1427,7 @@
       <c r="M29" s="6"/>
       <c r="N29" s="10"/>
       <c r="O29" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="P29" s="9">
         <v>1</v>
@@ -1446,7 +1446,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="6"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
@@ -1455,7 +1455,7 @@
       <c r="M30" s="6"/>
       <c r="N30" s="10"/>
       <c r="O30" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="P30" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
Added SARS-CoV-2 report (in chronological order of Double Check)
</commit_message>
<xml_diff>
--- a/doc/Reports_Permissions.xlsx
+++ b/doc/Reports_Permissions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web\webroot\test\files\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5382EE5-818E-4A0B-895F-EA3BB60431D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D13644-CD32-4625-BD82-6798A7EBD0D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>#</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>report_13.php</t>
+  </si>
+  <si>
+    <t>SARS</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,12 +607,12 @@
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="13" width="15.85546875" customWidth="1"/>
-    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="11" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -631,14 +634,15 @@
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="11"/>
+      <c r="O1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -672,10 +676,13 @@
       <c r="M2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="10"/>
+      <c r="N2" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="O2" s="10"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P2" s="10"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -695,17 +702,18 @@
       <c r="K3" s="2"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="3"/>
+      <c r="O3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -725,15 +733,16 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="3" t="s">
+      <c r="N4" s="6"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -753,15 +762,16 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="3" t="s">
+      <c r="N5" s="6"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -781,15 +791,16 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="3" t="s">
+      <c r="N6" s="6"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P6" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -809,15 +820,16 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="3" t="s">
+      <c r="N7" s="6"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -837,15 +849,16 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="3" t="s">
+      <c r="N8" s="6"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -865,15 +878,16 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="3" t="s">
+      <c r="N9" s="2"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="P9" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -893,15 +907,16 @@
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="3" t="s">
+      <c r="N10" s="2"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="P10" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -921,15 +936,16 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="3" t="s">
+      <c r="N11" s="3"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P11" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -949,15 +965,16 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="3" t="s">
+      <c r="N12" s="6"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P12" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -977,15 +994,16 @@
       <c r="K13" s="2"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="3" t="s">
+      <c r="N13" s="6"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="P13" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1005,15 +1023,16 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="3" t="s">
+      <c r="N14" s="6"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P14" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1033,15 +1052,16 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="3" t="s">
+      <c r="N15" s="6"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1061,15 +1081,16 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="3" t="s">
+      <c r="N16" s="6"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1089,15 +1110,16 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="3" t="s">
+      <c r="N17" s="6"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P17" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1117,15 +1139,16 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="3" t="s">
+      <c r="N18" s="6"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P18" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1145,15 +1168,16 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="3" t="s">
+      <c r="N19" s="6"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P19" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1173,15 +1197,16 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="3" t="s">
+      <c r="N20" s="6"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P20" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1201,15 +1226,16 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="3" t="s">
+      <c r="N21" s="6"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P21" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1229,15 +1255,16 @@
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="3" t="s">
+      <c r="N22" s="6"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P22" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1257,15 +1284,16 @@
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="3" t="s">
+      <c r="N23" s="6"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P23" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1285,15 +1313,16 @@
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="3" t="s">
+      <c r="N24" s="6"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P24" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1313,15 +1342,16 @@
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="3" t="s">
+      <c r="N25" s="6"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P25" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1341,15 +1371,16 @@
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="3" t="s">
+      <c r="N26" s="6"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P26" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1369,15 +1400,16 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="3" t="s">
+      <c r="N27" s="6"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P27" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1397,15 +1429,16 @@
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="3" t="s">
+      <c r="N28" s="6"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P28" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1425,15 +1458,16 @@
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="3" t="s">
+      <c r="N29" s="6"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P29" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1453,15 +1487,16 @@
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="3" t="s">
+      <c r="N30" s="6"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P30" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1481,15 +1516,16 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="3" t="s">
+      <c r="N31" s="6"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P31" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1509,15 +1545,16 @@
       <c r="K32" s="3"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="3" t="s">
+      <c r="N32" s="6"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P32" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1537,15 +1574,16 @@
       <c r="K33" s="3"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="3" t="s">
+      <c r="N33" s="6"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P33" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q33" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1565,15 +1603,16 @@
       <c r="K34" s="3"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="3" t="s">
+      <c r="N34" s="6"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P34" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q34" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1593,15 +1632,16 @@
       <c r="K35" s="3"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="3" t="s">
+      <c r="N35" s="6"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P35" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q35" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1619,15 +1659,16 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
-      <c r="N36" s="10" t="s">
+      <c r="N36" s="6"/>
+      <c r="O36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="O36" s="1"/>
-      <c r="P36">
+      <c r="P36" s="1"/>
+      <c r="Q36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1645,13 +1686,14 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="1"/>
-      <c r="P37">
+      <c r="N37" s="6"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="1"/>
+      <c r="Q37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1669,15 +1711,16 @@
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
-      <c r="N38" s="10" t="s">
+      <c r="N38" s="6"/>
+      <c r="O38" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O38" s="1"/>
-      <c r="P38">
+      <c r="P38" s="1"/>
+      <c r="Q38">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1695,13 +1738,14 @@
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="1"/>
-      <c r="P39">
+      <c r="N39" s="6"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="1"/>
+      <c r="Q39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1719,13 +1763,14 @@
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="1"/>
-      <c r="P40">
+      <c r="N40" s="6"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="1"/>
+      <c r="Q40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1743,13 +1788,14 @@
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="1"/>
-      <c r="P41">
+      <c r="N41" s="6"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="1"/>
+      <c r="Q41">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1767,13 +1813,14 @@
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="1"/>
-      <c r="P42">
+      <c r="N42" s="6"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="1"/>
+      <c r="Q42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1791,13 +1838,14 @@
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="1"/>
-      <c r="P43">
+      <c r="N43" s="6"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="1"/>
+      <c r="Q43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1815,15 +1863,16 @@
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
-      <c r="N44" s="10" t="s">
+      <c r="N44" s="6"/>
+      <c r="O44" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O44" s="1"/>
-      <c r="P44">
+      <c r="P44" s="1"/>
+      <c r="Q44">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1841,13 +1890,14 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="1"/>
-      <c r="P45">
+      <c r="N45" s="6"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="1"/>
+      <c r="Q45">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1865,13 +1915,14 @@
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="1"/>
-      <c r="P46">
+      <c r="N46" s="6"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="1"/>
+      <c r="Q46">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1889,13 +1940,14 @@
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="1"/>
-      <c r="P47">
+      <c r="N47" s="6"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="1"/>
+      <c r="Q47">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1913,13 +1965,14 @@
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="1"/>
-      <c r="P48">
+      <c r="N48" s="6"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="1"/>
+      <c r="Q48">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1937,15 +1990,16 @@
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
-      <c r="N49" s="7" t="s">
+      <c r="N49" s="6"/>
+      <c r="O49" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O49" s="1"/>
-      <c r="P49">
+      <c r="P49" s="1"/>
+      <c r="Q49">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1963,15 +2017,16 @@
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
-      <c r="N50" s="10" t="s">
+      <c r="N50" s="6"/>
+      <c r="O50" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O50" s="1"/>
-      <c r="P50">
+      <c r="P50" s="1"/>
+      <c r="Q50">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1989,13 +2044,14 @@
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="1"/>
-      <c r="P51">
+      <c r="N51" s="6"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="1"/>
+      <c r="Q51">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2013,13 +2069,14 @@
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
-      <c r="N52" s="10"/>
-      <c r="O52" s="1"/>
-      <c r="P52">
+      <c r="N52" s="6"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="1"/>
+      <c r="Q52">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2037,13 +2094,14 @@
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
-      <c r="N53" s="10"/>
-      <c r="O53" s="1"/>
-      <c r="P53">
+      <c r="N53" s="6"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="1"/>
+      <c r="Q53">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2061,15 +2119,16 @@
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
-      <c r="N54" s="10" t="s">
+      <c r="N54" s="6"/>
+      <c r="O54" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O54" s="1"/>
-      <c r="P54">
+      <c r="P54" s="1"/>
+      <c r="Q54">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2087,13 +2146,14 @@
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
-      <c r="N55" s="10"/>
-      <c r="O55" s="1"/>
-      <c r="P55">
+      <c r="N55" s="6"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="1"/>
+      <c r="Q55">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2111,13 +2171,14 @@
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
       <c r="M56" s="6"/>
-      <c r="N56" s="10"/>
-      <c r="O56" s="1"/>
-      <c r="P56">
+      <c r="N56" s="6"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="1"/>
+      <c r="Q56">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2135,13 +2196,14 @@
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
       <c r="M57" s="6"/>
-      <c r="N57" s="10"/>
-      <c r="O57" s="1"/>
-      <c r="P57">
+      <c r="N57" s="6"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="1"/>
+      <c r="Q57">
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2159,13 +2221,14 @@
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
       <c r="M58" s="6"/>
-      <c r="N58" s="10"/>
-      <c r="O58" s="1"/>
-      <c r="P58">
+      <c r="N58" s="6"/>
+      <c r="O58" s="10"/>
+      <c r="P58" s="1"/>
+      <c r="Q58">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2183,13 +2246,14 @@
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
       <c r="M59" s="6"/>
-      <c r="N59" s="10"/>
-      <c r="O59" s="1"/>
-      <c r="P59">
+      <c r="N59" s="6"/>
+      <c r="O59" s="10"/>
+      <c r="P59" s="1"/>
+      <c r="Q59">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2207,13 +2271,14 @@
       <c r="K60" s="6"/>
       <c r="L60" s="6"/>
       <c r="M60" s="6"/>
-      <c r="N60" s="10"/>
-      <c r="O60" s="1"/>
-      <c r="P60">
+      <c r="N60" s="6"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="1"/>
+      <c r="Q60">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2231,13 +2296,14 @@
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
       <c r="M61" s="6"/>
-      <c r="N61" s="10"/>
-      <c r="O61" s="1"/>
-      <c r="P61">
+      <c r="N61" s="6"/>
+      <c r="O61" s="10"/>
+      <c r="P61" s="1"/>
+      <c r="Q61">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2255,11 +2321,12 @@
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
-      <c r="N62" s="7" t="s">
+      <c r="N62" s="6"/>
+      <c r="O62" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O62" s="1"/>
-      <c r="P62">
+      <c r="P62" s="1"/>
+      <c r="Q62">
         <v>8</v>
       </c>
     </row>
@@ -2270,23 +2337,23 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P63">
-    <sortCondition ref="P3:P63"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Q63">
+    <sortCondition ref="Q3:Q63"/>
     <sortCondition ref="B3:B63"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="N54:N61"/>
-    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="O54:O61"/>
+    <mergeCell ref="P1:P2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:M1"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="N3:N35"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="N38:N43"/>
-    <mergeCell ref="N44:N48"/>
-    <mergeCell ref="N50:N53"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="O3:O35"/>
+    <mergeCell ref="O36:O37"/>
+    <mergeCell ref="O38:O43"/>
+    <mergeCell ref="O44:O48"/>
+    <mergeCell ref="O50:O53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Reports of user Seda (id=208) became like user ArturMartirosyan (id=26)
</commit_message>
<xml_diff>
--- a/doc/Reports_Permissions.xlsx
+++ b/doc/Reports_Permissions.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web\webroot\test\files\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D13644-CD32-4625-BD82-6798A7EBD0D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54B823A-D64D-4EBD-AA30-D628B4B50CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
   <si>
     <t>#</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>SARS</t>
+  </si>
+  <si>
+    <t>Seda</t>
   </si>
 </sst>
 </file>
@@ -593,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,19 +1017,19 @@
         <v>36</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="10"/>
       <c r="P14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q14" s="9">
         <v>1</v>
@@ -1648,22 +1651,26 @@
       <c r="B36" s="3">
         <v>208</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="C36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="P36" s="1"/>
+      <c r="P36" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="Q36">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
New users applies for report with new design
</commit_message>
<xml_diff>
--- a/doc/Reports_Permissions.xlsx
+++ b/doc/Reports_Permissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web\webroot\test\files\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54B823A-D64D-4EBD-AA30-D628B4B50CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B74070C-1CB9-474B-9E4D-B7019C4D072F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
   <si>
     <t>#</t>
   </si>
@@ -229,6 +229,24 @@
   </si>
   <si>
     <t>Seda</t>
+  </si>
+  <si>
+    <t>Anush</t>
+  </si>
+  <si>
+    <t>Nara</t>
+  </si>
+  <si>
+    <t>Liar</t>
+  </si>
+  <si>
+    <t>Ani</t>
+  </si>
+  <si>
+    <t>Inga_bac</t>
+  </si>
+  <si>
+    <t>Razmik</t>
   </si>
 </sst>
 </file>
@@ -594,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,9 +1725,11 @@
       <c r="B38" s="3">
         <v>22</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="C38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -1722,7 +1742,9 @@
       <c r="O38" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="P38" s="1"/>
+      <c r="P38" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="Q38">
         <v>3</v>
       </c>
@@ -1734,8 +1756,10 @@
       <c r="B39" s="3">
         <v>36</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="6"/>
+      <c r="C39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -1747,7 +1771,9 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="10"/>
-      <c r="P39" s="1"/>
+      <c r="P39" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="Q39">
         <v>3</v>
       </c>
@@ -1759,7 +1785,9 @@
       <c r="B40" s="3">
         <v>152</v>
       </c>
-      <c r="C40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -1784,9 +1812,11 @@
       <c r="B41" s="3">
         <v>220</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="C41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -1797,7 +1827,9 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="10"/>
-      <c r="P41" s="1"/>
+      <c r="P41" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="Q41">
         <v>3</v>
       </c>
@@ -1809,8 +1841,10 @@
       <c r="B42" s="3">
         <v>242</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="6"/>
+      <c r="C42" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="2"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -1822,7 +1856,9 @@
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="O42" s="10"/>
-      <c r="P42" s="1"/>
+      <c r="P42" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="Q42">
         <v>3</v>
       </c>
@@ -1834,9 +1870,11 @@
       <c r="B43" s="3">
         <v>466</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="C43" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -1847,7 +1885,9 @@
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
       <c r="O43" s="10"/>
-      <c r="P43" s="1"/>
+      <c r="P43" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="Q43">
         <v>3</v>
       </c>
@@ -2342,6 +2382,63 @@
       <c r="B65" s="4" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="9"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="9"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="9"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="9"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="9"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="9"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="9"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="9"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="9"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="9"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="9"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="9"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="9"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="9"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="9"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="9"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="9"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="9"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Q63">

</xml_diff>

<commit_message>
Created Reports menu for Sevada (id = 732)
</commit_message>
<xml_diff>
--- a/doc/Reports_Permissions.xlsx
+++ b/doc/Reports_Permissions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web\webroot\test\files\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B74070C-1CB9-474B-9E4D-B7019C4D072F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41F19A6-11EC-4797-BE98-D27C9AE95EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t>#</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>Razmik</t>
+  </si>
+  <si>
+    <t>Sevada</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -305,11 +308,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -331,6 +371,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,7 +664,7 @@
   <dimension ref="A1:Q88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +773,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="P3" s="3" t="s">
@@ -755,7 +804,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
-      <c r="O4" s="10"/>
+      <c r="O4" s="13"/>
       <c r="P4" s="3" t="s">
         <v>59</v>
       </c>
@@ -784,7 +833,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
-      <c r="O5" s="10"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="3" t="s">
         <v>60</v>
       </c>
@@ -813,7 +862,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
-      <c r="O6" s="10"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="3" t="s">
         <v>61</v>
       </c>
@@ -842,7 +891,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
-      <c r="O7" s="10"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="3" t="s">
         <v>61</v>
       </c>
@@ -871,7 +920,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
-      <c r="O8" s="10"/>
+      <c r="O8" s="13"/>
       <c r="P8" s="3" t="s">
         <v>61</v>
       </c>
@@ -900,7 +949,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="10"/>
+      <c r="O9" s="13"/>
       <c r="P9" s="3" t="s">
         <v>62</v>
       </c>
@@ -929,7 +978,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="10"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="3" t="s">
         <v>65</v>
       </c>
@@ -958,7 +1007,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="10"/>
+      <c r="O11" s="13"/>
       <c r="P11" s="3" t="s">
         <v>60</v>
       </c>
@@ -987,7 +1036,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="10"/>
+      <c r="O12" s="13"/>
       <c r="P12" s="3" t="s">
         <v>60</v>
       </c>
@@ -1016,7 +1065,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="10"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="3" t="s">
         <v>63</v>
       </c>
@@ -1045,7 +1094,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
-      <c r="O14" s="10"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="3" t="s">
         <v>58</v>
       </c>
@@ -1074,7 +1123,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
-      <c r="O15" s="10"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="3" t="s">
         <v>59</v>
       </c>
@@ -1103,7 +1152,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="10"/>
+      <c r="O16" s="13"/>
       <c r="P16" s="3" t="s">
         <v>59</v>
       </c>
@@ -1132,7 +1181,7 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="10"/>
+      <c r="O17" s="13"/>
       <c r="P17" s="3" t="s">
         <v>61</v>
       </c>
@@ -1161,7 +1210,7 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
-      <c r="O18" s="10"/>
+      <c r="O18" s="13"/>
       <c r="P18" s="3" t="s">
         <v>60</v>
       </c>
@@ -1190,7 +1239,7 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
-      <c r="O19" s="10"/>
+      <c r="O19" s="13"/>
       <c r="P19" s="3" t="s">
         <v>64</v>
       </c>
@@ -1219,7 +1268,7 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
-      <c r="O20" s="10"/>
+      <c r="O20" s="13"/>
       <c r="P20" s="3" t="s">
         <v>64</v>
       </c>
@@ -1248,7 +1297,7 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="10"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="3" t="s">
         <v>60</v>
       </c>
@@ -1277,7 +1326,7 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="10"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="3" t="s">
         <v>61</v>
       </c>
@@ -1306,7 +1355,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
-      <c r="O23" s="10"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="3" t="s">
         <v>61</v>
       </c>
@@ -1335,7 +1384,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
-      <c r="O24" s="10"/>
+      <c r="O24" s="13"/>
       <c r="P24" s="3" t="s">
         <v>60</v>
       </c>
@@ -1364,7 +1413,7 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
-      <c r="O25" s="10"/>
+      <c r="O25" s="13"/>
       <c r="P25" s="3" t="s">
         <v>60</v>
       </c>
@@ -1393,7 +1442,7 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
-      <c r="O26" s="10"/>
+      <c r="O26" s="13"/>
       <c r="P26" s="3" t="s">
         <v>64</v>
       </c>
@@ -1422,7 +1471,7 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
-      <c r="O27" s="10"/>
+      <c r="O27" s="13"/>
       <c r="P27" s="3" t="s">
         <v>64</v>
       </c>
@@ -1451,7 +1500,7 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
-      <c r="O28" s="10"/>
+      <c r="O28" s="13"/>
       <c r="P28" s="3" t="s">
         <v>59</v>
       </c>
@@ -1480,7 +1529,7 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
-      <c r="O29" s="10"/>
+      <c r="O29" s="13"/>
       <c r="P29" s="3" t="s">
         <v>64</v>
       </c>
@@ -1509,7 +1558,7 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
-      <c r="O30" s="10"/>
+      <c r="O30" s="13"/>
       <c r="P30" s="3" t="s">
         <v>64</v>
       </c>
@@ -1538,7 +1587,7 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
-      <c r="O31" s="10"/>
+      <c r="O31" s="13"/>
       <c r="P31" s="3" t="s">
         <v>59</v>
       </c>
@@ -1567,7 +1616,7 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
-      <c r="O32" s="10"/>
+      <c r="O32" s="13"/>
       <c r="P32" s="3" t="s">
         <v>61</v>
       </c>
@@ -1596,7 +1645,7 @@
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
-      <c r="O33" s="10"/>
+      <c r="O33" s="13"/>
       <c r="P33" s="3" t="s">
         <v>61</v>
       </c>
@@ -1625,7 +1674,7 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
-      <c r="O34" s="10"/>
+      <c r="O34" s="13"/>
       <c r="P34" s="3" t="s">
         <v>60</v>
       </c>
@@ -1654,7 +1703,7 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
-      <c r="O35" s="10"/>
+      <c r="O35" s="13"/>
       <c r="P35" s="3" t="s">
         <v>61</v>
       </c>
@@ -1663,73 +1712,75 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>34</v>
+      <c r="A36" s="3">
+        <v>61</v>
       </c>
       <c r="B36" s="3">
-        <v>208</v>
+        <v>732</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+      <c r="I36" s="6"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="P36" s="3" t="s">
-        <v>58</v>
+      <c r="L36" s="3"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q36">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="3">
-        <v>422</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
+        <v>208</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="1"/>
+      <c r="O37" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="Q37">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="3">
-        <v>22</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+        <v>422</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -1739,28 +1790,24 @@
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
-      <c r="O38" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="O38" s="10"/>
+      <c r="P38" s="1"/>
       <c r="Q38">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="6"/>
+      <c r="E39" s="2"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -1770,9 +1817,11 @@
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
-      <c r="O39" s="10"/>
+      <c r="O39" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="P39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q39">
         <v>3</v>
@@ -1780,15 +1829,15 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="3">
-        <v>152</v>
+        <v>36</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -1800,23 +1849,25 @@
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="O40" s="10"/>
-      <c r="P40" s="1"/>
+      <c r="P40" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="Q40">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="3">
-        <v>220</v>
+        <v>152</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -1827,25 +1878,23 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="10"/>
-      <c r="P41" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="P41" s="1"/>
       <c r="Q41">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="3">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="6"/>
+      <c r="E42" s="2"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
@@ -1857,7 +1906,7 @@
       <c r="N42" s="6"/>
       <c r="O42" s="10"/>
       <c r="P42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q42">
         <v>3</v>
@@ -1865,16 +1914,16 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="3">
-        <v>466</v>
+        <v>242</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -1886,7 +1935,7 @@
       <c r="N43" s="6"/>
       <c r="O43" s="10"/>
       <c r="P43" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q43">
         <v>3</v>
@@ -1894,14 +1943,16 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="3">
-        <v>69</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+        <v>466</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -1911,20 +1962,20 @@
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
-      <c r="O44" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="P44" s="1"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="Q44">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="3">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="6"/>
@@ -1938,7 +1989,9 @@
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
-      <c r="O45" s="10"/>
+      <c r="O45" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="P45" s="1"/>
       <c r="Q45">
         <v>4</v>
@@ -1946,10 +1999,10 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="3">
-        <v>184</v>
+        <v>132</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="6"/>
@@ -1971,10 +2024,10 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="3">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="6"/>
@@ -1996,10 +2049,10 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="3">
-        <v>278</v>
+        <v>212</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="6"/>
@@ -2021,10 +2074,10 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="3">
-        <v>390</v>
+        <v>278</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="6"/>
@@ -2038,20 +2091,18 @@
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
-      <c r="O49" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="O49" s="10"/>
       <c r="P49" s="1"/>
       <c r="Q49">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="3">
-        <v>1</v>
+        <v>390</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="6"/>
@@ -2065,20 +2116,20 @@
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
-      <c r="O50" s="10" t="s">
-        <v>13</v>
+      <c r="O50" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="P50" s="1"/>
       <c r="Q50">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="6"/>
@@ -2092,7 +2143,9 @@
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
       <c r="N51" s="6"/>
-      <c r="O51" s="10"/>
+      <c r="O51" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="P51" s="1"/>
       <c r="Q51">
         <v>6</v>
@@ -2100,10 +2153,10 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="6"/>
@@ -2125,10 +2178,10 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="3">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="6"/>
@@ -2150,10 +2203,10 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="3">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="6"/>
@@ -2167,20 +2220,18 @@
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
-      <c r="O54" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="O54" s="10"/>
       <c r="P54" s="1"/>
       <c r="Q54">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="3">
-        <v>448</v>
+        <v>10</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="6"/>
@@ -2194,7 +2245,9 @@
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
-      <c r="O55" s="10"/>
+      <c r="O55" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="P55" s="1"/>
       <c r="Q55">
         <v>7</v>
@@ -2202,10 +2255,10 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="3">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="6"/>
@@ -2227,10 +2280,10 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="3">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="6"/>
@@ -2252,10 +2305,10 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="3">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="6"/>
@@ -2277,10 +2330,10 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="3">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="6"/>
@@ -2302,10 +2355,10 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="3">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="6"/>
@@ -2327,10 +2380,10 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="3">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="6"/>
@@ -2352,10 +2405,10 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="3">
-        <v>170</v>
+        <v>460</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="6"/>
@@ -2369,11 +2422,36 @@
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
       <c r="N62" s="6"/>
-      <c r="O62" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="O62" s="10"/>
       <c r="P62" s="1"/>
       <c r="Q62">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>60</v>
+      </c>
+      <c r="B63" s="3">
+        <v>170</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P63" s="1"/>
+      <c r="Q63">
         <v>8</v>
       </c>
     </row>
@@ -2446,18 +2524,18 @@
     <sortCondition ref="B3:B63"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="O54:O61"/>
+    <mergeCell ref="O55:O62"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:N1"/>
     <mergeCell ref="O1:O2"/>
-    <mergeCell ref="O3:O35"/>
-    <mergeCell ref="O36:O37"/>
-    <mergeCell ref="O38:O43"/>
-    <mergeCell ref="O44:O48"/>
-    <mergeCell ref="O50:O53"/>
+    <mergeCell ref="O37:O38"/>
+    <mergeCell ref="O39:O44"/>
+    <mergeCell ref="O45:O49"/>
+    <mergeCell ref="O51:O54"/>
+    <mergeCell ref="O3:O36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>